<commit_message>
some stuff that doesn't work
</commit_message>
<xml_diff>
--- a/Many2Many.xlsx
+++ b/Many2Many.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Category</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Product_ID</t>
   </si>
   <si>
-    <t>ProductsCategory</t>
-  </si>
-  <si>
     <t>Air Jordans</t>
   </si>
   <si>
@@ -82,6 +79,12 @@
   </si>
   <si>
     <t>Adidas</t>
+  </si>
+  <si>
+    <t>CategorizedProducts</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -547,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -564,7 +567,7 @@
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1"/>
       <c r="K1" s="1" t="s">
@@ -611,16 +614,16 @@
         <v>199.5</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
       </c>
       <c r="H3">
         <v>2000</v>
@@ -632,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -643,16 +646,16 @@
         <v>2.99</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
       </c>
       <c r="H4">
         <v>2000</v>
@@ -664,7 +667,7 @@
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -676,6 +679,11 @@
       </c>
       <c r="I5">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>